<commit_message>
added lib/api.js and corrected number input fields
</commit_message>
<xml_diff>
--- a/BUSINESS PLAN - BWI.xlsx
+++ b/BUSINESS PLAN - BWI.xlsx
@@ -1825,7 +1825,7 @@
         </is>
       </c>
       <c r="C7" s="104" t="n">
-        <v>1200000</v>
+        <v>1300000</v>
       </c>
       <c r="D7" s="70" t="n"/>
       <c r="E7" s="70" t="n"/>
@@ -1846,7 +1846,7 @@
         <v/>
       </c>
       <c r="D8" s="94" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E8" s="73" t="n">
         <v>1</v>
@@ -1926,7 +1926,7 @@
         </is>
       </c>
       <c r="C13" s="95" t="n">
-        <v>116.62</v>
+        <v>118</v>
       </c>
       <c r="D13" s="70" t="n"/>
       <c r="E13" s="70" t="n"/>

</xml_diff>

<commit_message>
atualizado next.config.js para ter o output
</commit_message>
<xml_diff>
--- a/BUSINESS PLAN - BWI.xlsx
+++ b/BUSINESS PLAN - BWI.xlsx
@@ -1825,7 +1825,7 @@
         </is>
       </c>
       <c r="C7" s="104" t="n">
-        <v>1300000</v>
+        <v>1400000</v>
       </c>
       <c r="D7" s="70" t="n"/>
       <c r="E7" s="70" t="n"/>
@@ -1943,7 +1943,7 @@
         </is>
       </c>
       <c r="C14" s="95" t="n">
-        <v>212</v>
+        <v>250</v>
       </c>
       <c r="D14" s="70" t="n"/>
       <c r="E14" s="70" t="n"/>

</xml_diff>